<commit_message>
Updated Excel Sheet and added comments
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth Kharade\SimplicityStudio\v5_workspace\ecen5823-assignment6-parthkharade\questions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446F3D87-0D6F-492F-B658-E4A78FFF0A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -25,13 +34,100 @@
     <t>Use this column to denote if BT stack events cause your state machine to advance, you can put an X in the cell to note this. Drawing a bubble diagram of your state machine might also be a good idea 👍.</t>
   </si>
   <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>LCD Display State</t>
+  </si>
+  <si>
+    <t>Advances State Machine</t>
+  </si>
+  <si>
+    <t>Commands called in response to event</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Events Common to Slaves/Clients</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_system_boot_id</t>
+  </si>
+  <si>
+    <t>This event is generated on stack boot up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can also document in column D values that need to be saved in response to receiving BT stack events. </t>
+  </si>
+  <si>
+    <t>sl_bt_scanner_set_mode()</t>
+  </si>
+  <si>
+    <t>Set phy to 1M and mode to passive scanning</t>
+  </si>
+  <si>
+    <t>sl_bt_scanner_set_timing()</t>
+  </si>
+  <si>
+    <t>Set phy to 1M, scan interval to 50ms and scan window to 25ms</t>
+  </si>
+  <si>
+    <t>sl_bt_connection_set_default_parameters()</t>
+  </si>
+  <si>
+    <t>See the assignment document for these values</t>
+  </si>
+  <si>
+    <t>sl_bt_scanner_start()</t>
+  </si>
+  <si>
+    <t>You should start and stop scanning just like you did with advertising for a Server.</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_connection_opened_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_connection_closed_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_system_soft_timer_id</t>
+  </si>
+  <si>
+    <t>This event indicates that a soft timer has expired.</t>
+  </si>
+  <si>
+    <t>Events only for Masters/Clients</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_scanner_scan_report_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_procedure_completed_id</t>
+  </si>
+  <si>
+    <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not build your state machine into your  handle_ble_event() function! Instead build a new state machine for A7. </t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_service_id</t>
+  </si>
+  <si>
+    <t>A GATT service in the remote GATT database was discovered</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_characteristic_id</t>
+  </si>
+  <si>
+    <t>A GATT characteristic in the remote GATT database was discovered</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_characteristic_value_id</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
       <t xml:space="preserve">Commands that may be useful:
 </t>
     </r>
@@ -41,20 +137,12 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">sl_bt_gatt_discover_primary_services_by_uuid()
-</t>
+      <t>sl_bt_gatt_discover_primary_services_by_uuid()
+sl_bt_gatt_discover_characteristics_by_uuid()</t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sl_bt_gatt_discover_characteristics_by_uuid()</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -64,127 +152,89 @@
     </r>
   </si>
   <si>
-    <t>Event</t>
-  </si>
-  <si>
-    <t>LCD Display State</t>
-  </si>
-  <si>
-    <t>Advances State Machine</t>
-  </si>
-  <si>
-    <t>Commands called in response to event</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Events Common to Slaves/Clients</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_system_boot_id</t>
-  </si>
-  <si>
-    <t>This event is generated on stack boot up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can also document in column D values that need to be saved in response to receiving BT stack events. </t>
-  </si>
-  <si>
-    <t>sl_bt_scanner_set_mode()</t>
-  </si>
-  <si>
-    <t>Set phy to 1M and mode to passive scanning</t>
-  </si>
-  <si>
-    <t>sl_bt_scanner_set_timing()</t>
-  </si>
-  <si>
-    <t>Set phy to 1M, scan interval to 50ms and scan window to 25ms</t>
-  </si>
-  <si>
-    <t>sl_bt_connection_set_default_parameters()</t>
-  </si>
-  <si>
-    <t>See the assignment document for these values</t>
-  </si>
-  <si>
-    <t>sl_bt_scanner_start()</t>
-  </si>
-  <si>
-    <t>You should start and stop scanning just like you did with advertising for a Server.</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_connection_opened_id</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_connection_closed_id</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_system_soft_timer_id</t>
-  </si>
-  <si>
-    <t>This event indicates that a soft timer has expired.</t>
-  </si>
-  <si>
-    <t>Events only for Masters/Clients</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_scanner_scan_report_id</t>
-  </si>
-  <si>
-    <t>Received for advertising or scan response packets generated by: sl_bt_scanner_start().
-Is the bd_addr, packet_type and address_type what we expect for our Server? If yes:
-   sl_bt_scanner_stop()
-   sl_bt_connection_open()</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_procedure_completed_id</t>
-  </si>
-  <si>
-    <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not build your state machine into your  handle_ble_event() function! Instead build a new state machine for A7. </t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_service_id</t>
-  </si>
-  <si>
-    <t>A GATT service in the remote GATT database was discovered</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_characteristic_id</t>
-  </si>
-  <si>
-    <t>A GATT characteristic in the remote GATT database was discovered</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_characteristic_value_id</t>
-  </si>
-  <si>
-    <t>If an indication or notification has been enabled for a characteristic, this event is triggered whenever an indication or notification is received from the remote GATT server.
+    <t>sl_bt_gatt_discover_primary_services_by_uuid()</t>
+  </si>
+  <si>
+    <t>displayUpdate()</t>
+  </si>
+  <si>
+    <t>Save connection_handle</t>
+  </si>
+  <si>
+    <t>Values to save</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_discover_characteristics_by_uuid() on first event instance</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_set_characteristic_notification() on second event instance</t>
+  </si>
+  <si>
+    <t>save gatt_htm service handle</t>
+  </si>
+  <si>
+    <t>save gatt_htm_characterisitc handle</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If an indication or notification has been enabled for a characteristic, this event is triggered whenever an indication or notification is received from the remote GATT server.
 Is the characteristic handle and att_opcode we expect? If yes: 
-   sl_bt_gatt_send_characteristic_confirmation()</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>sl_bt_gatt_send_characteristic_confirmation()</t>
+    </r>
+  </si>
+  <si>
+    <t>Convert and display temperature value.</t>
+  </si>
+  <si>
+    <r>
+      <t>Received for advertising or scan response packets generated by: sl_bt_scanner_start().
+Is the bd_addr, packet_type and address_type what we expect for our Server? If yes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+sl_bt_connection_open()</t>
+  </si>
+  <si>
+    <t>sl_bt_scanner_stop()</t>
+  </si>
+  <si>
+    <t>This event occurs three times. The third time it just advances the state machine. No function to call</t>
+  </si>
+  <si>
+    <t>STATE DIAGRAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="13"/>
@@ -197,7 +247,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -218,9 +268,58 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -329,80 +428,82 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="29">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,28 +512,151 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff2236ff"/>
-      <rgbColor rgb="ff4d8f72"/>
-      <rgbColor rgb="ff4d8f72"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF2236FF"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127635</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>240030</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F34B94F7-443D-D032-7BE4-429DD665C9DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="127635" y="11995785"/>
+          <a:ext cx="7343775" cy="4006215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -634,7 +858,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -653,7 +877,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -683,7 +907,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -709,7 +933,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -735,7 +959,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -761,7 +985,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -787,7 +1011,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -813,7 +1037,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -839,7 +1063,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -865,7 +1089,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -891,7 +1115,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,9 +1128,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -923,7 +1153,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -942,7 +1172,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,7 +1198,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -994,7 +1224,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +1250,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1046,7 +1276,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1072,7 +1302,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1098,7 +1328,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1124,7 +1354,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1150,7 +1380,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1176,7 +1406,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,9 +1419,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1205,7 +1441,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1224,7 +1460,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,7 +1490,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1280,7 +1516,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1306,7 +1542,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1332,7 +1568,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1358,7 +1594,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1384,7 +1620,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1410,7 +1646,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1436,7 +1672,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1462,7 +1698,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1475,352 +1711,457 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.8516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="26.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.55" customHeight="1">
+    <row r="1" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" ht="12.05" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" ht="119.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" t="s" s="9">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="119.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" s="6"/>
+      <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="F3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" ht="12.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s" s="6">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="D4" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="9">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="9">
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s" s="9">
+    </row>
+    <row r="5" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" ht="13.75" customHeight="1">
-      <c r="A5" t="s" s="10">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" ht="26.75" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" t="s" s="11">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" t="s" s="14">
+      <c r="G6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s" s="15">
+    </row>
+    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" t="s" s="17">
+      <c r="G7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s" s="15">
+    </row>
+    <row r="8" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" ht="13.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" t="s" s="17">
+      <c r="G8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s" s="18">
+    </row>
+    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" t="s" s="17">
+      <c r="G9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s" s="15">
+    </row>
+    <row r="10" spans="1:7" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" ht="26.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" t="s" s="17">
+      <c r="G10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s" s="15">
+    </row>
+    <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" t="s" s="20">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" t="s" s="20">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" t="s" s="20">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" t="s" s="21">
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" t="s" s="10">
+      <c r="B18" s="4"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19" ht="78.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" t="s" s="20">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" t="s" s="21">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="19"/>
-    </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" ht="39.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" t="s" s="20">
+      <c r="G22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" t="s" s="21">
+    </row>
+    <row r="23" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F21" t="s" s="15">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" t="s" s="20">
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" t="s" s="21">
+      <c r="C28" s="16"/>
+      <c r="D28" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" t="s" s="20">
+      <c r="G28" s="16"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" t="s" s="21">
-        <v>35</v>
-      </c>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" ht="65.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" t="s" s="20">
-        <v>36</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" t="s" s="21">
-        <v>37</v>
-      </c>
-      <c r="F27" s="19"/>
-    </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="C30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="35" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>